<commit_message>
update cape BOM typo
</commit_message>
<xml_diff>
--- a/Robotics Cape Reference Documents/SD-101D Robotics Cape BOM.xlsx
+++ b/Robotics Cape Reference Documents/SD-101D Robotics Cape BOM.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Dropbox\SD-101D Robotics Cape\Internal  Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="180" windowWidth="14160" windowHeight="13065"/>
   </bookViews>
   <sheets>
     <sheet name="Rev D BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="238">
   <si>
     <t>IMU</t>
   </si>
@@ -160,9 +165,6 @@
     <t>24-LSSOP</t>
   </si>
   <si>
-    <t>http://www.samsungsem.com/servlet/FileDownload?type=spec&amp;file=CL10B222KB8NCNC.pdf</t>
-  </si>
-  <si>
     <t>Assembly Labor</t>
   </si>
   <si>
@@ -211,9 +213,6 @@
     <t>100k Ohm resistor</t>
   </si>
   <si>
-    <t>2.2nF 50v Cap</t>
-  </si>
-  <si>
     <t>Lithium Charge IC</t>
   </si>
   <si>
@@ -469,12 +468,6 @@
     <t>http://www.digikey.com/product-detail/en/CL05A104MP5NNNC/1276-1443-1-ND/3889529</t>
   </si>
   <si>
-    <t>CL05B222KB5NNNC</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/CL05B222KB5NNNC/1276-1054-1-ND/3889140</t>
-  </si>
-  <si>
     <t>ON Semi</t>
   </si>
   <si>
@@ -500,12 +493,6 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/BM04B-SRSS-TB(LF)(SN)/455-1790-1-ND/926861</t>
-  </si>
-  <si>
-    <t>qty 1000, 1wk</t>
-  </si>
-  <si>
-    <t>qty 200, 5days</t>
   </si>
   <si>
     <t>4pcb.com</t>
@@ -636,9 +623,6 @@
     <t>Strawson Design 2015    Not for Public Disclosure</t>
   </si>
   <si>
-    <t>D4</t>
-  </si>
-  <si>
     <t>160 Ohm Resistor</t>
   </si>
   <si>
@@ -651,9 +635,6 @@
     <t>R49</t>
   </si>
   <si>
-    <t>65K Ohm resistor</t>
-  </si>
-  <si>
     <t>DO-214AA</t>
   </si>
   <si>
@@ -672,9 +653,6 @@
     <t>MPU-9250</t>
   </si>
   <si>
-    <t>C21</t>
-  </si>
-  <si>
     <t>6.3uH inductor 3A</t>
   </si>
   <si>
@@ -711,27 +689,15 @@
     <t>C4, C10</t>
   </si>
   <si>
-    <t>C1, C2, C6, C9, C8, C13, C14,  C15, C17, C18, C19, C22, C24</t>
-  </si>
-  <si>
     <t>C3, C5, C7, C12, C16, C20, C23, C25, C26</t>
   </si>
   <si>
     <t>R47</t>
   </si>
   <si>
-    <t>R3, R9, R15, R16, R17, R18, R20, R26, R35, R46, R44</t>
-  </si>
-  <si>
     <t>CHG, GRN, D5, D6, D7</t>
   </si>
   <si>
-    <t>R10, R11, R12, R13, R14, R25, R36, R37, R38, R39, R40, R41, R42, R43, R50, R51, R52, R53, R54, R55, R56, R57, R7</t>
-  </si>
-  <si>
-    <t>R5, R6, R48, R8</t>
-  </si>
-  <si>
     <t>MPS</t>
   </si>
   <si>
@@ -741,7 +707,55 @@
     <t>https://www.monolithicpower.com/DesktopModules/DocumentManage/API/Document/GetDocument?id=3323</t>
   </si>
   <si>
-    <t>R28, R27, R34</t>
+    <t>C1, C2, C6, C8, C9, C13, C14,  C15, C17, C18, C19, C21, C22, C24</t>
+  </si>
+  <si>
+    <t>R5, R6, R8, R48</t>
+  </si>
+  <si>
+    <t>R27, R28, R34</t>
+  </si>
+  <si>
+    <t>R3, R9, R15, R16, R17, R18, R20, R26, R35, R44, R46</t>
+  </si>
+  <si>
+    <t>R7, R10, R11, R12, R13, R14, R25, R36, R37, R38, R39, R40, R41, R42, R43, R50, R51, R52, R53, R54, R55, R56, R57</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>RC1005F6492CS</t>
+  </si>
+  <si>
+    <t>64.9K Ohm resistor</t>
+  </si>
+  <si>
+    <t>0402 SMD</t>
+  </si>
+  <si>
+    <t>CL05A105KO5NNNC</t>
+  </si>
+  <si>
+    <t>PREC023DAAN-RC</t>
+  </si>
+  <si>
+    <t>Sullins</t>
+  </si>
+  <si>
+    <t>TSW-108-08-F-T-RA</t>
+  </si>
+  <si>
+    <t>Samtec</t>
+  </si>
+  <si>
+    <t>http://suddendocs.samtec.com/catalog_english/tsw_th.pdf</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/TSW-108-08-T-S-RA/SAM1051-08-ND/1102416?WT.srch=1</t>
+  </si>
+  <si>
+    <t>Conformal Coating</t>
   </si>
 </sst>
 </file>
@@ -829,12 +843,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -860,6 +868,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1004,7 +1018,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1132,7 +1146,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1160,13 +1174,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -1179,37 +1193,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1272,7 +1295,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1307,7 +1330,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1521,8 +1544,8 @@
   </sheetPr>
   <dimension ref="A2:N81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1544,54 +1567,54 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
-        <v>197</v>
-      </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
+      <c r="A2" s="88" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
       <c r="M2" s="8"/>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
-        <v>198</v>
-      </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
+      <c r="A3" s="88" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="88"/>
       <c r="M3" s="14"/>
       <c r="N3" s="15"/>
     </row>
     <row r="4" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="85"/>
-      <c r="B4" s="85"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="85"/>
+      <c r="A4" s="90"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
       <c r="M4" s="12"/>
       <c r="N4" s="1"/>
     </row>
@@ -1603,22 +1626,22 @@
     <row r="6" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>54</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>55</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>38</v>
@@ -1652,7 +1675,7 @@
       <c r="J7" s="21"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="4" t="s">
@@ -1662,17 +1685,15 @@
     <row r="8" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>162</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="E8" s="24"/>
       <c r="F8" s="25" t="s">
         <v>11</v>
       </c>
@@ -1680,16 +1701,15 @@
         <v>1</v>
       </c>
       <c r="H8" s="25">
-        <v>2.2400000000000002</v>
+        <v>0</v>
       </c>
       <c r="I8" s="25">
-        <f>G8*H8</f>
-        <v>2.2400000000000002</v>
+        <v>0</v>
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="49"/>
       <c r="L8" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M8" s="42"/>
       <c r="N8" s="4" t="s">
@@ -1698,60 +1718,54 @@
     </row>
     <row r="9" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
-      <c r="B9" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="36" t="s">
-        <v>165</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>163</v>
-      </c>
-      <c r="F9" s="32" t="s">
+      <c r="B9" s="85" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="87"/>
+    </row>
+    <row r="10" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="52"/>
+      <c r="D10" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="36"/>
+      <c r="F10" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G10" s="32">
         <v>1</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H10" s="32">
         <v>0</v>
       </c>
-      <c r="I9" s="32">
-        <f>G9*H9</f>
+      <c r="I10" s="32">
+        <f>G10*H10</f>
         <v>0</v>
       </c>
-      <c r="J9" s="32"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="M9" s="43"/>
-      <c r="N9" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="I10" s="43">
-        <f>SUM(I8:I9)</f>
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="M10" s="6"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="M10" s="43"/>
       <c r="N10" s="4" t="s">
         <v>28</v>
       </c>
@@ -1764,114 +1778,99 @@
       <c r="E11" s="17"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="H11" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="43">
+        <f>SUM(I8:I10)</f>
+        <v>0</v>
+      </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M11" s="6"/>
       <c r="N11" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="78" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="20"/>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
-      <c r="F12" s="21"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
       <c r="L12" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="M12" s="9"/>
+        <v>110</v>
+      </c>
+      <c r="M12" s="6"/>
       <c r="N12" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="72" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="55" t="s">
-        <v>231</v>
-      </c>
-      <c r="D13" s="65" t="s">
-        <v>220</v>
-      </c>
-      <c r="E13" s="65" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="55" t="s">
-        <v>221</v>
-      </c>
-      <c r="G13" s="25">
-        <v>1</v>
-      </c>
-      <c r="H13" s="55">
-        <v>1.37</v>
-      </c>
-      <c r="I13" s="55">
-        <f t="shared" ref="I13:I18" si="0">G13*H13</f>
-        <v>1.37</v>
-      </c>
-      <c r="J13" s="25"/>
-      <c r="K13" s="26" t="s">
-        <v>232</v>
-      </c>
-      <c r="L13" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="M13" s="28" t="s">
-        <v>233</v>
-      </c>
+    <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="78" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="M13" s="9"/>
       <c r="N13" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B14" s="72" t="s">
-        <v>175</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="80" t="s">
-        <v>170</v>
-      </c>
-      <c r="E14" s="63" t="s">
-        <v>171</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="G14" s="6">
+        <v>64</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>218</v>
+      </c>
+      <c r="D14" s="65" t="s">
+        <v>211</v>
+      </c>
+      <c r="E14" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="55" t="s">
+        <v>212</v>
+      </c>
+      <c r="G14" s="25">
         <v>1</v>
       </c>
-      <c r="H14" s="21">
-        <v>0.34</v>
-      </c>
-      <c r="I14" s="21">
-        <f>G14*H14</f>
-        <v>0.34</v>
-      </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="M14" s="30" t="s">
-        <v>174</v>
+      <c r="H14" s="55">
+        <v>1.37</v>
+      </c>
+      <c r="I14" s="55">
+        <f t="shared" ref="I14:I19" si="0">G14*H14</f>
+        <v>1.37</v>
+      </c>
+      <c r="J14" s="25"/>
+      <c r="K14" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="L14" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="M14" s="28" t="s">
+        <v>220</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>28</v>
@@ -1879,39 +1878,39 @@
     </row>
     <row r="15" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B15" s="72" t="s">
-        <v>116</v>
+        <v>169</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="D15" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="79" t="s">
+        <v>164</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>165</v>
+      </c>
+      <c r="F15" s="21" t="s">
         <v>166</v>
-      </c>
-      <c r="E15" s="63" t="s">
-        <v>115</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>167</v>
       </c>
       <c r="G15" s="6">
         <v>1</v>
       </c>
       <c r="H15" s="21">
-        <v>0.37</v>
+        <v>0.34</v>
       </c>
       <c r="I15" s="21">
         <f>G15*H15</f>
-        <v>0.37</v>
+        <v>0.34</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="M15" s="30" t="s">
         <v>168</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="M15" s="30" t="s">
-        <v>169</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>28</v>
@@ -1919,349 +1918,360 @@
     </row>
     <row r="16" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B16" s="72" t="s">
-        <v>8</v>
+        <v>114</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="D16" s="63" t="s">
-        <v>210</v>
+        <v>160</v>
       </c>
       <c r="E16" s="63" t="s">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>72</v>
+        <v>161</v>
       </c>
       <c r="G16" s="6">
         <v>1</v>
       </c>
       <c r="H16" s="21">
+        <v>0.37</v>
+      </c>
+      <c r="I16" s="21">
+        <f>G16*H16</f>
+        <v>0.37</v>
+      </c>
+      <c r="J16" s="6"/>
+      <c r="K16" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="M16" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="63" t="s">
+        <v>202</v>
+      </c>
+      <c r="E17" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1</v>
+      </c>
+      <c r="H17" s="21">
         <v>3.7</v>
       </c>
-      <c r="I16" s="21">
+      <c r="I17" s="21">
         <f t="shared" si="0"/>
         <v>3.7</v>
       </c>
-      <c r="J16" s="6"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" ht="16.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="72" t="s">
+      <c r="J17" s="6"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" ht="16.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" s="63" t="s">
-        <v>118</v>
-      </c>
-      <c r="E17" s="63" t="s">
-        <v>88</v>
-      </c>
-      <c r="F17" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="G17" s="6">
+      <c r="C18" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18" s="6">
         <v>1</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H18" s="21">
         <v>0.36899999999999999</v>
       </c>
-      <c r="I17" s="21">
+      <c r="I18" s="21">
         <f t="shared" si="0"/>
         <v>0.36899999999999999</v>
       </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="L17" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="M17" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="72" t="s">
+      <c r="J18" s="6"/>
+      <c r="K18" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="M18" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="D18" s="63" t="s">
+      <c r="C19" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="63" t="s">
-        <v>89</v>
-      </c>
-      <c r="F18" s="21" t="s">
+      <c r="E19" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G19" s="6">
         <v>2</v>
       </c>
-      <c r="H18" s="21">
+      <c r="H19" s="21">
         <v>1.21</v>
       </c>
-      <c r="I18" s="21">
+      <c r="I19" s="21">
         <f t="shared" si="0"/>
         <v>2.42</v>
       </c>
-      <c r="J18" s="6"/>
-      <c r="K18" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="L18" s="9" t="s">
+      <c r="J19" s="6"/>
+      <c r="K19" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="M19" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="72" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" s="58" t="s">
+        <v>187</v>
+      </c>
+      <c r="D20" s="62" t="s">
+        <v>177</v>
+      </c>
+      <c r="E20" s="62" t="s">
+        <v>186</v>
+      </c>
+      <c r="F20" t="s">
+        <v>178</v>
+      </c>
+      <c r="G20" s="50">
+        <v>1</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0.42</v>
+      </c>
+      <c r="I20" s="21">
+        <f>G20*H20</f>
+        <v>0.42</v>
+      </c>
+      <c r="J20" s="4"/>
+      <c r="K20" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="73" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="G21" s="32">
+        <v>1</v>
+      </c>
+      <c r="H21" s="54">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="I21" s="54">
+        <f>G21*H21</f>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54" t="s">
+        <v>126</v>
+      </c>
+      <c r="L21" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="M21" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="M18" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="N18" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="72" t="s">
-        <v>194</v>
-      </c>
-      <c r="C19" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="D19" s="62" t="s">
-        <v>183</v>
-      </c>
-      <c r="E19" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="F19" t="s">
-        <v>184</v>
-      </c>
-      <c r="G19" s="50">
-        <v>1</v>
-      </c>
-      <c r="H19" s="4">
-        <v>0.42</v>
-      </c>
-      <c r="I19" s="21">
-        <f>G19*H19</f>
-        <v>0.42</v>
-      </c>
-      <c r="J19" s="4"/>
-      <c r="K19" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="L19" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="N19" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="73" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" s="54" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" s="64" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="F20" s="54" t="s">
-        <v>113</v>
-      </c>
-      <c r="G20" s="32">
-        <v>1</v>
-      </c>
-      <c r="H20" s="54">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="I20" s="54">
-        <f>G20*H20</f>
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="J20" s="54"/>
-      <c r="K20" s="54" t="s">
-        <v>128</v>
-      </c>
-      <c r="L20" s="54" t="s">
-        <v>112</v>
-      </c>
-      <c r="M20" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="N20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="H21" s="73" t="s">
-        <v>78</v>
-      </c>
-      <c r="I21" s="74">
-        <f>SUM(I13:I20)</f>
+      <c r="N21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="H22" s="73" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="74">
+        <f>SUM(I14:I21)</f>
         <v>11.228999999999999</v>
       </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="M21" s="6"/>
-      <c r="N21" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="62"/>
-      <c r="E22" s="66"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M22" s="6"/>
       <c r="N22" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:14" ht="27.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="75" t="s">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="62"/>
+      <c r="E23" s="66"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="M23" s="6"/>
+      <c r="N23" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" ht="27.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="55" t="s">
-        <v>135</v>
-      </c>
-      <c r="D23" s="65" t="s">
-        <v>149</v>
-      </c>
-      <c r="E23" s="69" t="s">
-        <v>224</v>
-      </c>
-      <c r="F23" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="G23" s="25">
+      <c r="C24" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" s="65" t="s">
+        <v>147</v>
+      </c>
+      <c r="E24" s="69" t="s">
+        <v>221</v>
+      </c>
+      <c r="F24" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="G24" s="25">
         <v>13</v>
       </c>
-      <c r="H23" s="55">
+      <c r="H24" s="55">
         <v>5.3600000000000002E-3</v>
       </c>
-      <c r="I23" s="55">
-        <f>G23*H23</f>
+      <c r="I24" s="55">
+        <f>G24*H24</f>
         <v>6.9680000000000006E-2</v>
       </c>
-      <c r="J23" s="25"/>
-      <c r="K23" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="L23" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="M23" s="28" t="s">
+      <c r="J24" s="25"/>
+      <c r="K24" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="L24" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="M24" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="N23" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" ht="27.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="72" t="s">
-        <v>222</v>
-      </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="70" t="s">
-        <v>223</v>
-      </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="6">
+      <c r="N24" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" ht="27.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="72" t="s">
+        <v>213</v>
+      </c>
+      <c r="C25" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>230</v>
+      </c>
+      <c r="E25" s="70" t="s">
+        <v>214</v>
+      </c>
+      <c r="F25" s="58" t="s">
+        <v>229</v>
+      </c>
+      <c r="G25" s="6">
         <v>2</v>
       </c>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="30"/>
-    </row>
-    <row r="25" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="72" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="D25" s="63" t="s">
-        <v>151</v>
-      </c>
-      <c r="E25" s="70" t="s">
-        <v>211</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="G25" s="6">
-        <v>1</v>
-      </c>
-      <c r="H25" s="21">
-        <v>3.5999999999999999E-3</v>
-      </c>
-      <c r="I25" s="21">
+      <c r="H25" s="58">
+        <v>4.3E-3</v>
+      </c>
+      <c r="I25" s="55">
         <f>G25*H25</f>
-        <v>3.5999999999999999E-3</v>
+        <v>8.6E-3</v>
       </c>
       <c r="J25" s="6"/>
-      <c r="K25" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="L25" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="M25" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="N25" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="K25" s="7"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="30"/>
     </row>
     <row r="26" spans="2:14" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B26" s="72" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D26" s="63" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E26" s="70" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G26" s="6">
         <v>9</v>
@@ -2275,13 +2285,13 @@
       </c>
       <c r="J26" s="6"/>
       <c r="K26" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M26" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>28</v>
@@ -2289,19 +2299,19 @@
     </row>
     <row r="27" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B27" s="73" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="54" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D27" s="64" t="s">
         <v>37</v>
       </c>
       <c r="E27" s="71" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F27" s="54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G27" s="32">
         <v>1</v>
@@ -2318,7 +2328,7 @@
         <v>36</v>
       </c>
       <c r="L27" s="34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M27" s="35" t="s">
         <v>26</v>
@@ -2331,16 +2341,16 @@
       <c r="D28" s="62"/>
       <c r="E28" s="66"/>
       <c r="H28" s="56" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I28" s="57">
-        <f>SUM(I23:I27)</f>
-        <v>0.85728000000000015</v>
+        <f>SUM(I24:I27)</f>
+        <v>0.86228000000000016</v>
       </c>
       <c r="J28" s="21"/>
       <c r="K28" s="21"/>
       <c r="L28" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M28" s="9"/>
       <c r="N28" s="4" t="s">
@@ -2349,14 +2359,14 @@
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D29" s="62"/>
       <c r="E29" s="66"/>
       <c r="J29" s="6"/>
       <c r="K29" s="7"/>
       <c r="L29" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M29" s="9"/>
       <c r="N29" s="4" t="s">
@@ -2368,13 +2378,13 @@
         <v>32</v>
       </c>
       <c r="C30" s="55" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D30" s="65" t="s">
         <v>40</v>
       </c>
       <c r="E30" s="60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F30" s="55" t="s">
         <v>31</v>
@@ -2391,13 +2401,13 @@
       </c>
       <c r="J30" s="25"/>
       <c r="K30" s="26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L30" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M30" s="28" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>28</v>
@@ -2405,50 +2415,55 @@
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="72" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="D31" s="80" t="s">
-        <v>209</v>
+        <v>133</v>
+      </c>
+      <c r="D31" s="79" t="s">
+        <v>201</v>
       </c>
       <c r="E31" s="61" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G31" s="6">
         <v>3</v>
       </c>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
+      <c r="H31" s="58">
+        <v>0.05</v>
+      </c>
+      <c r="I31" s="55">
+        <f>G31*H31</f>
+        <v>0.15000000000000002</v>
+      </c>
       <c r="J31" s="6"/>
       <c r="K31" s="7"/>
       <c r="L31" s="9"/>
       <c r="M31" s="28" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="72" t="s">
         <v>39</v>
       </c>
       <c r="C32" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" s="63" t="s">
         <v>135</v>
       </c>
-      <c r="D32" s="63" t="s">
-        <v>137</v>
-      </c>
-      <c r="E32" s="70" t="s">
-        <v>201</v>
+      <c r="E32" s="68" t="s">
+        <v>194</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G32" s="6">
         <v>7</v>
@@ -2462,13 +2477,13 @@
       </c>
       <c r="J32" s="6"/>
       <c r="K32" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L32" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M32" s="28" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>28</v>
@@ -2476,19 +2491,19 @@
     </row>
     <row r="33" spans="2:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="72" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D33" s="63" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E33" s="61" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G33" s="6">
         <v>11</v>
@@ -2497,18 +2512,18 @@
         <v>2.3E-3</v>
       </c>
       <c r="I33" s="21">
-        <f t="shared" si="1"/>
+        <f>G33*H33</f>
         <v>2.53E-2</v>
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="L33" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M33" s="28" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>28</v>
@@ -2516,19 +2531,19 @@
     </row>
     <row r="34" spans="2:14" ht="62.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B34" s="72" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D34" s="63" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E34" s="61" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G34" s="6">
         <v>23</v>
@@ -2542,13 +2557,13 @@
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M34" s="28" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>28</v>
@@ -2556,19 +2571,19 @@
     </row>
     <row r="35" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B35" s="72" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D35" s="63" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E35" s="61" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G35" s="6">
         <v>4</v>
@@ -2582,13 +2597,13 @@
       </c>
       <c r="J35" s="6"/>
       <c r="K35" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L35" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M35" s="28" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>28</v>
@@ -2596,19 +2611,19 @@
     </row>
     <row r="36" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B36" s="72" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D36" s="63" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E36" s="61" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G36" s="6">
         <v>3</v>
@@ -2622,13 +2637,13 @@
       </c>
       <c r="J36" s="6"/>
       <c r="K36" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="L36" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M36" s="28" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>28</v>
@@ -2636,28 +2651,35 @@
     </row>
     <row r="37" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B37" s="72" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>135</v>
-      </c>
-      <c r="D37" s="63"/>
+        <v>133</v>
+      </c>
+      <c r="D37" s="63" t="s">
+        <v>227</v>
+      </c>
       <c r="E37" s="61" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="G37" s="82">
+        <v>128</v>
+      </c>
+      <c r="G37" s="80">
         <v>1</v>
       </c>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
+      <c r="H37" s="58">
+        <v>3.9199999999999999E-3</v>
+      </c>
+      <c r="I37" s="58">
+        <f>G37*H37</f>
+        <v>3.9199999999999999E-3</v>
+      </c>
       <c r="J37" s="6"/>
       <c r="K37" s="7"/>
       <c r="L37" s="9"/>
       <c r="M37" s="28" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>28</v>
@@ -2665,19 +2687,19 @@
     </row>
     <row r="38" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B38" s="73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" s="54" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D38" s="64" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E38" s="67" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="F38" s="54" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G38" s="32">
         <v>1</v>
@@ -2691,13 +2713,13 @@
       </c>
       <c r="J38" s="32"/>
       <c r="K38" s="33" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L38" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="M38" s="86" t="s">
-        <v>208</v>
+        <v>110</v>
+      </c>
+      <c r="M38" s="81" t="s">
+        <v>200</v>
       </c>
       <c r="N38" s="4" t="s">
         <v>28</v>
@@ -2707,16 +2729,16 @@
       <c r="D39" s="62"/>
       <c r="E39" s="66"/>
       <c r="H39" s="73" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I39" s="74">
         <f>SUM(I30:I38)</f>
-        <v>0.19968000000000002</v>
+        <v>0.35360000000000003</v>
       </c>
       <c r="J39" s="21"/>
       <c r="K39" s="21"/>
       <c r="L39" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M39" s="9"/>
       <c r="N39" s="4" t="s">
@@ -2725,14 +2747,14 @@
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D40" s="62"/>
       <c r="E40" s="66"/>
       <c r="J40" s="21"/>
       <c r="K40" s="21"/>
       <c r="L40" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M40" s="9"/>
       <c r="N40" s="4" t="s">
@@ -2744,13 +2766,13 @@
         <v>13</v>
       </c>
       <c r="C41" s="55" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D41" s="65" t="s">
         <v>44</v>
       </c>
       <c r="E41" s="60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F41" s="55" t="s">
         <v>17</v>
@@ -2770,7 +2792,7 @@
         <v>45</v>
       </c>
       <c r="L41" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M41" s="37" t="s">
         <v>46</v>
@@ -2784,18 +2806,18 @@
         <v>13</v>
       </c>
       <c r="C42" t="s">
-        <v>187</v>
-      </c>
-      <c r="D42" s="80" t="s">
-        <v>188</v>
-      </c>
-      <c r="E42" s="79" t="s">
-        <v>199</v>
+        <v>181</v>
+      </c>
+      <c r="D42" s="79" t="s">
+        <v>182</v>
+      </c>
+      <c r="E42" s="91" t="s">
+        <v>226</v>
       </c>
       <c r="F42" s="59" t="s">
-        <v>205</v>
-      </c>
-      <c r="G42" s="82">
+        <v>197</v>
+      </c>
+      <c r="G42" s="80">
         <v>1</v>
       </c>
       <c r="H42" s="47">
@@ -2807,13 +2829,13 @@
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="L42" s="9" t="s">
         <v>28</v>
       </c>
       <c r="M42" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="N42" s="4" t="s">
         <v>28</v>
@@ -2824,13 +2846,13 @@
         <v>18</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D43" s="63" t="s">
         <v>20</v>
       </c>
       <c r="E43" s="61" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="F43" s="21" t="s">
         <v>31</v>
@@ -2850,7 +2872,7 @@
         <v>21</v>
       </c>
       <c r="L43" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M43" s="29" t="s">
         <v>19</v>
@@ -2864,13 +2886,13 @@
         <v>22</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D44" s="63" t="s">
         <v>23</v>
       </c>
       <c r="E44" s="61" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F44" s="21" t="s">
         <v>31</v>
@@ -2890,7 +2912,7 @@
         <v>24</v>
       </c>
       <c r="L44" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M44" s="29" t="s">
         <v>25</v>
@@ -2901,19 +2923,19 @@
     </row>
     <row r="45" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B45" s="72" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C45" s="58" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D45" s="63" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E45" s="61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G45" s="6">
         <v>2</v>
@@ -2927,13 +2949,13 @@
       </c>
       <c r="J45" s="6"/>
       <c r="K45" s="7" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="L45" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M45" s="30" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>28</v>
@@ -2941,19 +2963,19 @@
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B46" s="72" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C46" s="58" t="s">
-        <v>157</v>
-      </c>
-      <c r="D46" s="80" t="s">
-        <v>217</v>
+        <v>153</v>
+      </c>
+      <c r="D46" s="79" t="s">
+        <v>208</v>
       </c>
       <c r="E46" s="66" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F46" s="58" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="G46" s="50">
         <v>1</v>
@@ -2967,13 +2989,13 @@
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="L46" s="9" t="s">
         <v>28</v>
       </c>
       <c r="M46" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>28</v>
@@ -2981,24 +3003,24 @@
     </row>
     <row r="47" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B47" s="73" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C47" s="54" t="s">
-        <v>207</v>
-      </c>
-      <c r="D47" s="87" t="s">
-        <v>179</v>
+        <v>199</v>
+      </c>
+      <c r="D47" s="82" t="s">
+        <v>173</v>
       </c>
       <c r="E47" s="67" t="s">
-        <v>206</v>
-      </c>
-      <c r="F47" s="88" t="s">
-        <v>176</v>
-      </c>
-      <c r="G47" s="89">
+        <v>198</v>
+      </c>
+      <c r="F47" s="83" t="s">
+        <v>170</v>
+      </c>
+      <c r="G47" s="84">
         <v>1</v>
       </c>
-      <c r="H47" s="88">
+      <c r="H47" s="83">
         <v>0.22</v>
       </c>
       <c r="I47" s="54">
@@ -3007,13 +3029,13 @@
       </c>
       <c r="J47" s="32"/>
       <c r="K47" s="33" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="L47" s="34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M47" s="38" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>28</v>
@@ -3023,7 +3045,7 @@
       <c r="D48" s="62"/>
       <c r="E48" s="66"/>
       <c r="H48" s="73" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I48" s="74">
         <f>SUM(I41:I47)</f>
@@ -3032,7 +3054,7 @@
       <c r="J48" s="6"/>
       <c r="K48" s="7"/>
       <c r="L48" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M48" s="9"/>
       <c r="N48" s="4" t="s">
@@ -3041,14 +3063,14 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B49" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D49" s="62"/>
       <c r="E49" s="66"/>
       <c r="J49" s="6"/>
       <c r="K49" s="7"/>
       <c r="L49" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M49" s="22"/>
       <c r="N49" s="4" t="s">
@@ -3060,13 +3082,13 @@
         <v>2</v>
       </c>
       <c r="C50" s="55" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D50" s="65" t="s">
         <v>4</v>
       </c>
       <c r="E50" s="60" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F50" s="55" t="s">
         <v>27</v>
@@ -3100,16 +3122,16 @@
         <v>41</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D51" s="63" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E51" s="61" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F51" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G51" s="6">
         <v>4</v>
@@ -3123,13 +3145,13 @@
       </c>
       <c r="J51" s="6"/>
       <c r="K51" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L51" s="9" t="s">
         <v>28</v>
       </c>
       <c r="M51" s="30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>28</v>
@@ -3137,12 +3159,16 @@
     </row>
     <row r="52" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B52" s="72" t="s">
-        <v>93</v>
-      </c>
-      <c r="C52" s="58"/>
-      <c r="D52" s="81"/>
+        <v>91</v>
+      </c>
+      <c r="C52" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="D52" s="92" t="s">
+        <v>231</v>
+      </c>
       <c r="E52" s="61" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F52" s="21" t="s">
         <v>27</v>
@@ -3151,11 +3177,11 @@
         <v>2</v>
       </c>
       <c r="H52" s="21">
-        <v>0.58099999999999996</v>
+        <v>0.35</v>
       </c>
       <c r="I52" s="21">
         <f t="shared" si="3"/>
-        <v>1.1619999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="J52" s="11"/>
       <c r="K52" s="7" t="s">
@@ -3173,12 +3199,16 @@
     </row>
     <row r="53" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B53" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="C53" s="21"/>
-      <c r="D53" s="63"/>
+        <v>154</v>
+      </c>
+      <c r="C53" s="58" t="s">
+        <v>234</v>
+      </c>
+      <c r="D53" s="63" t="s">
+        <v>233</v>
+      </c>
       <c r="E53" s="61" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F53" s="21" t="s">
         <v>27</v>
@@ -3187,32 +3217,36 @@
         <v>1</v>
       </c>
       <c r="H53" s="21">
-        <v>0.51519999999999999</v>
+        <v>0.35</v>
       </c>
       <c r="I53" s="21">
         <f>G53*H53</f>
-        <v>0.51519999999999999</v>
+        <v>0.35</v>
       </c>
       <c r="J53" s="11"/>
-      <c r="K53" s="7"/>
+      <c r="K53" s="7" t="s">
+        <v>236</v>
+      </c>
       <c r="L53" s="9"/>
-      <c r="M53" s="30"/>
+      <c r="M53" s="30" t="s">
+        <v>235</v>
+      </c>
       <c r="N53" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B54" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D54" s="63" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E54" s="61" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F54" s="21" t="s">
         <v>27</v>
@@ -3229,13 +3263,13 @@
       </c>
       <c r="J54" s="11"/>
       <c r="K54" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L54" s="9" t="s">
         <v>28</v>
       </c>
       <c r="M54" s="30" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N54" s="4" t="s">
         <v>28</v>
@@ -3243,19 +3277,19 @@
     </row>
     <row r="55" spans="1:14" ht="32.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B55" s="72" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D55" s="63" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E55" s="61" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G55" s="6">
         <v>8</v>
@@ -3269,13 +3303,13 @@
       </c>
       <c r="J55" s="11"/>
       <c r="K55" s="7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="L55" s="9" t="s">
         <v>28</v>
       </c>
       <c r="M55" s="53" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>28</v>
@@ -3283,19 +3317,19 @@
     </row>
     <row r="56" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B56" s="72" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D56" s="63" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E56" s="61" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="F56" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G56" s="6">
         <v>4</v>
@@ -3323,16 +3357,16 @@
     </row>
     <row r="57" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B57" s="72" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D57" s="63" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E57" s="61" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F57" s="21" t="s">
         <v>27</v>
@@ -3349,13 +3383,13 @@
       </c>
       <c r="J57" s="11"/>
       <c r="K57" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L57" s="9" t="s">
         <v>28</v>
       </c>
       <c r="M57" s="30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>28</v>
@@ -3363,16 +3397,16 @@
     </row>
     <row r="58" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B58" s="73" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C58" s="54" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D58" s="64" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E58" s="67" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F58" s="54" t="s">
         <v>27</v>
@@ -3389,13 +3423,13 @@
       </c>
       <c r="J58" s="44"/>
       <c r="K58" s="33" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L58" s="34" t="s">
         <v>28</v>
       </c>
       <c r="M58" s="38" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N58" s="4" t="s">
         <v>28</v>
@@ -3409,11 +3443,11 @@
       <c r="F59" s="39"/>
       <c r="G59" s="40"/>
       <c r="H59" s="76" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I59" s="43">
         <f>SUM(I50:I58)</f>
-        <v>9.2176000000000009</v>
+        <v>8.5904000000000007</v>
       </c>
       <c r="J59" s="21"/>
       <c r="K59" s="7"/>
@@ -3449,16 +3483,16 @@
       <c r="D61" s="17"/>
       <c r="E61" s="61"/>
       <c r="F61" s="77" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G61" s="46">
-        <f>SUM(G13:G58)</f>
-        <v>130</v>
+        <f>SUM(G14:G58)</f>
+        <v>129</v>
       </c>
       <c r="H61" s="6"/>
       <c r="I61" s="13">
-        <f>SUM(I10,I21,I28,I39,I48,I59)</f>
-        <v>25.462600000000002</v>
+        <f>SUM(I11,I22,I28,I39,I48,I59)</f>
+        <v>22.75432</v>
       </c>
       <c r="J61" s="19" t="s">
         <v>12</v>
@@ -3636,50 +3670,52 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K41" r:id="rId1"/>
-    <hyperlink ref="K23" r:id="rId2"/>
-    <hyperlink ref="M23" r:id="rId3"/>
+    <hyperlink ref="K24" r:id="rId2"/>
+    <hyperlink ref="M24" r:id="rId3"/>
     <hyperlink ref="M41" r:id="rId4"/>
     <hyperlink ref="K43" r:id="rId5"/>
     <hyperlink ref="K26" r:id="rId6"/>
     <hyperlink ref="M27" r:id="rId7"/>
     <hyperlink ref="K27" r:id="rId8"/>
-    <hyperlink ref="M18" r:id="rId9"/>
+    <hyperlink ref="M19" r:id="rId9"/>
     <hyperlink ref="M26" r:id="rId10"/>
-    <hyperlink ref="K25" r:id="rId11"/>
-    <hyperlink ref="M25" r:id="rId12"/>
-    <hyperlink ref="M43" r:id="rId13"/>
-    <hyperlink ref="K44" r:id="rId14"/>
-    <hyperlink ref="M50" r:id="rId15"/>
-    <hyperlink ref="K50" r:id="rId16"/>
-    <hyperlink ref="K51" r:id="rId17"/>
-    <hyperlink ref="M52" r:id="rId18"/>
-    <hyperlink ref="M51" r:id="rId19"/>
-    <hyperlink ref="K56" r:id="rId20"/>
-    <hyperlink ref="K57" r:id="rId21"/>
-    <hyperlink ref="M56" r:id="rId22"/>
-    <hyperlink ref="M57" r:id="rId23"/>
-    <hyperlink ref="M17" r:id="rId24"/>
-    <hyperlink ref="K17" r:id="rId25"/>
-    <hyperlink ref="M55" r:id="rId26"/>
-    <hyperlink ref="K55" r:id="rId27"/>
-    <hyperlink ref="K58" r:id="rId28"/>
-    <hyperlink ref="K20" r:id="rId29"/>
-    <hyperlink ref="K18" r:id="rId30"/>
-    <hyperlink ref="M15" r:id="rId31"/>
-    <hyperlink ref="K15" r:id="rId32"/>
-    <hyperlink ref="K30" r:id="rId33"/>
-    <hyperlink ref="M30" r:id="rId34"/>
-    <hyperlink ref="K32" r:id="rId35"/>
-    <hyperlink ref="K34" r:id="rId36"/>
-    <hyperlink ref="K14" r:id="rId37"/>
-    <hyperlink ref="M19" r:id="rId38"/>
-    <hyperlink ref="K19" r:id="rId39"/>
-    <hyperlink ref="K42" r:id="rId40"/>
-    <hyperlink ref="K47" r:id="rId41"/>
-    <hyperlink ref="M31:M38" r:id="rId42" display="http://www.samsungsem.com/global/support/library/product-catalog/__icsFiles/afieldfile/2015/01/12/CHIP_RESISTOR_150112_1.pdf"/>
+    <hyperlink ref="M43" r:id="rId11"/>
+    <hyperlink ref="K44" r:id="rId12"/>
+    <hyperlink ref="M50" r:id="rId13"/>
+    <hyperlink ref="K50" r:id="rId14"/>
+    <hyperlink ref="K51" r:id="rId15"/>
+    <hyperlink ref="M52" r:id="rId16"/>
+    <hyperlink ref="M51" r:id="rId17"/>
+    <hyperlink ref="K56" r:id="rId18"/>
+    <hyperlink ref="K57" r:id="rId19"/>
+    <hyperlink ref="M56" r:id="rId20"/>
+    <hyperlink ref="M57" r:id="rId21"/>
+    <hyperlink ref="M18" r:id="rId22"/>
+    <hyperlink ref="K18" r:id="rId23"/>
+    <hyperlink ref="M55" r:id="rId24"/>
+    <hyperlink ref="K55" r:id="rId25"/>
+    <hyperlink ref="K58" r:id="rId26"/>
+    <hyperlink ref="K21" r:id="rId27"/>
+    <hyperlink ref="K19" r:id="rId28"/>
+    <hyperlink ref="M16" r:id="rId29"/>
+    <hyperlink ref="K16" r:id="rId30"/>
+    <hyperlink ref="K30" r:id="rId31"/>
+    <hyperlink ref="M30" r:id="rId32"/>
+    <hyperlink ref="K32" r:id="rId33"/>
+    <hyperlink ref="K34" r:id="rId34"/>
+    <hyperlink ref="K15" r:id="rId35"/>
+    <hyperlink ref="M20" r:id="rId36"/>
+    <hyperlink ref="K20" r:id="rId37"/>
+    <hyperlink ref="K42" r:id="rId38"/>
+    <hyperlink ref="K47" r:id="rId39"/>
+    <hyperlink ref="M31:M38" r:id="rId40" display="http://www.samsungsem.com/global/support/library/product-catalog/__icsFiles/afieldfile/2015/01/12/CHIP_RESISTOR_150112_1.pdf"/>
+    <hyperlink ref="M47" r:id="rId41"/>
+    <hyperlink ref="M53" r:id="rId42"/>
+    <hyperlink ref="M54" r:id="rId43"/>
+    <hyperlink ref="K53" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="44" orientation="landscape" r:id="rId43"/>
+  <pageSetup scale="44" orientation="landscape" r:id="rId45"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="65" max="16383" man="1"/>
   </rowBreaks>

</xml_diff>